<commit_message>
6/9 Saving SheeData through streaming: Change the saving of a worksheet from "read attached DOM, modify DOM, will be auto-saved to part" to "read detached DOM, stream DOM to part." SampleSparklines was modified, because it now has namespace declarations directly in the root elements.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Sparklines/SampleSparklines.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Sparklines/SampleSparklines.xlsx
@@ -427,7 +427,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:worksheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
@@ -1342,7 +1342,7 @@
   <x:extLst>
     <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" lineWeight="0.75" type="line" dateAxis="0" displayEmptyCellsAs="span" markers="1" high="1" low="1" first="1" last="1" negative="1" displayXAxis="0" displayHidden="0" minAxisType="group" maxAxisType="group" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
+        <x14:sparklineGroup lineWeight="0.75" type="line" dateAxis="0" displayEmptyCellsAs="span" markers="1" high="1" low="1" first="1" last="1" negative="1" displayXAxis="0" displayHidden="0" minAxisType="group" maxAxisType="group" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
           <x14:colorSeries rgb="FF5F5F5F"/>
           <x14:colorNegative rgb="FFFFB620"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1366,7 +1366,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" lineWeight="0.75" type="line" dateAxis="0" displayEmptyCellsAs="span" markers="0" high="1" low="1" first="1" last="1" negative="0" displayXAxis="0" displayHidden="0" minAxisType="individual" maxAxisType="individual" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
+        <x14:sparklineGroup lineWeight="0.75" type="line" dateAxis="0" displayEmptyCellsAs="span" markers="0" high="1" low="1" first="1" last="1" negative="0" displayXAxis="0" displayHidden="0" minAxisType="individual" maxAxisType="individual" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
           <x14:colorSeries rgb="FF5687C2"/>
           <x14:colorNegative rgb="FFFFB620"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1390,7 +1390,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" manualMax="100" manualMin="-80" lineWeight="0.75" type="line" dateAxis="0" displayEmptyCellsAs="span" markers="1" high="0" low="0" first="0" last="0" negative="1" displayXAxis="0" displayHidden="0" minAxisType="custom" maxAxisType="custom" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
+        <x14:sparklineGroup manualMax="100" manualMin="-80" lineWeight="0.75" type="line" dateAxis="0" displayEmptyCellsAs="span" markers="1" high="0" low="0" first="0" last="0" negative="1" displayXAxis="0" displayHidden="0" minAxisType="custom" maxAxisType="custom" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
           <x14:colorSeries rgb="FFC6EFCE"/>
           <x14:colorNegative rgb="FFFFC7CE"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1414,7 +1414,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" lineWeight="0.75" type="line" dateAxis="1" displayEmptyCellsAs="span" markers="0" high="0" low="0" first="0" last="0" negative="0" displayXAxis="0" displayHidden="0" minAxisType="individual" maxAxisType="individual" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
+        <x14:sparklineGroup lineWeight="0.75" type="line" dateAxis="1" displayEmptyCellsAs="span" markers="0" high="0" low="0" first="0" last="0" negative="0" displayXAxis="0" displayHidden="0" minAxisType="individual" maxAxisType="individual" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
           <x14:colorSeries rgb="FF5F5F5F"/>
           <x14:colorNegative rgb="FFFFB620"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1439,7 +1439,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" lineWeight="2" type="line" dateAxis="0" displayEmptyCellsAs="span" markers="0" high="0" low="0" first="0" last="0" negative="0" displayXAxis="1" displayHidden="0" minAxisType="individual" maxAxisType="individual" rightToLeft="1" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
+        <x14:sparklineGroup lineWeight="2" type="line" dateAxis="0" displayEmptyCellsAs="span" markers="0" high="0" low="0" first="0" last="0" negative="0" displayXAxis="1" displayHidden="0" minAxisType="individual" maxAxisType="individual" rightToLeft="1" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
           <x14:colorSeries rgb="FF00B050"/>
           <x14:colorNegative rgb="FFFF0000"/>
           <x14:colorAxis rgb="FFFF0000"/>
@@ -1463,7 +1463,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" lineWeight="0.75" type="line" dateAxis="0" displayEmptyCellsAs="span" markers="0" high="0" low="0" first="1" last="1" negative="0" displayXAxis="0" displayHidden="0" minAxisType="individual" maxAxisType="individual" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
+        <x14:sparklineGroup lineWeight="0.75" type="line" dateAxis="0" displayEmptyCellsAs="span" markers="0" high="0" low="0" first="1" last="1" negative="0" displayXAxis="0" displayHidden="0" minAxisType="individual" maxAxisType="individual" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
           <x14:colorSeries rgb="FFC6EFCE"/>
           <x14:colorNegative rgb="FFFFC7CE"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -1494,7 +1494,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:worksheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
@@ -2417,7 +2417,7 @@
   <x:extLst>
     <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" lineWeight="0.75" type="column" dateAxis="0" displayEmptyCellsAs="span" markers="1" high="1" low="1" first="1" last="1" negative="1" displayXAxis="0" displayHidden="0" minAxisType="group" maxAxisType="group" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
+        <x14:sparklineGroup lineWeight="0.75" type="column" dateAxis="0" displayEmptyCellsAs="span" markers="1" high="1" low="1" first="1" last="1" negative="1" displayXAxis="0" displayHidden="0" minAxisType="group" maxAxisType="group" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
           <x14:colorSeries rgb="FF5F5F5F"/>
           <x14:colorNegative rgb="FFFFB620"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -2441,7 +2441,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" lineWeight="0.75" type="column" dateAxis="0" displayEmptyCellsAs="span" markers="0" high="1" low="1" first="1" last="1" negative="0" displayXAxis="0" displayHidden="0" minAxisType="individual" maxAxisType="individual" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
+        <x14:sparklineGroup lineWeight="0.75" type="column" dateAxis="0" displayEmptyCellsAs="span" markers="0" high="1" low="1" first="1" last="1" negative="0" displayXAxis="0" displayHidden="0" minAxisType="individual" maxAxisType="individual" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
           <x14:colorSeries rgb="FF5687C2"/>
           <x14:colorNegative rgb="FFFFB620"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -2465,7 +2465,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" manualMax="100" manualMin="-80" lineWeight="0.75" type="column" dateAxis="0" displayEmptyCellsAs="span" markers="1" high="0" low="0" first="0" last="0" negative="1" displayXAxis="0" displayHidden="0" minAxisType="custom" maxAxisType="custom" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
+        <x14:sparklineGroup manualMax="100" manualMin="-80" lineWeight="0.75" type="column" dateAxis="0" displayEmptyCellsAs="span" markers="1" high="0" low="0" first="0" last="0" negative="1" displayXAxis="0" displayHidden="0" minAxisType="custom" maxAxisType="custom" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
           <x14:colorSeries rgb="FFC6EFCE"/>
           <x14:colorNegative rgb="FFFFC7CE"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -2489,7 +2489,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" lineWeight="0.75" type="column" dateAxis="1" displayEmptyCellsAs="span" markers="0" high="0" low="0" first="0" last="0" negative="0" displayXAxis="0" displayHidden="0" minAxisType="individual" maxAxisType="individual" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
+        <x14:sparklineGroup lineWeight="0.75" type="column" dateAxis="1" displayEmptyCellsAs="span" markers="0" high="0" low="0" first="0" last="0" negative="0" displayXAxis="0" displayHidden="0" minAxisType="individual" maxAxisType="individual" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
           <x14:colorSeries rgb="FF5F5F5F"/>
           <x14:colorNegative rgb="FFFFB620"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -2514,7 +2514,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" lineWeight="2" type="column" dateAxis="0" displayEmptyCellsAs="span" markers="0" high="0" low="0" first="0" last="0" negative="0" displayXAxis="1" displayHidden="0" minAxisType="individual" maxAxisType="individual" rightToLeft="1" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
+        <x14:sparklineGroup lineWeight="2" type="column" dateAxis="0" displayEmptyCellsAs="span" markers="0" high="0" low="0" first="0" last="0" negative="0" displayXAxis="1" displayHidden="0" minAxisType="individual" maxAxisType="individual" rightToLeft="1" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
           <x14:colorSeries rgb="FF00B050"/>
           <x14:colorNegative rgb="FFFF0000"/>
           <x14:colorAxis rgb="FFFF0000"/>
@@ -2538,7 +2538,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" lineWeight="0.75" type="column" dateAxis="0" displayEmptyCellsAs="span" markers="0" high="0" low="0" first="1" last="1" negative="0" displayXAxis="0" displayHidden="0" minAxisType="individual" maxAxisType="individual" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
+        <x14:sparklineGroup lineWeight="0.75" type="column" dateAxis="0" displayEmptyCellsAs="span" markers="0" high="0" low="0" first="1" last="1" negative="0" displayXAxis="0" displayHidden="0" minAxisType="individual" maxAxisType="individual" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
           <x14:colorSeries rgb="FFC6EFCE"/>
           <x14:colorNegative rgb="FFFFC7CE"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -2569,7 +2569,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:worksheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
@@ -3492,7 +3492,7 @@
   <x:extLst>
     <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" lineWeight="0.75" type="stacked" dateAxis="0" displayEmptyCellsAs="span" markers="1" high="1" low="1" first="1" last="1" negative="1" displayXAxis="0" displayHidden="0" minAxisType="group" maxAxisType="group" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
+        <x14:sparklineGroup lineWeight="0.75" type="stacked" dateAxis="0" displayEmptyCellsAs="span" markers="1" high="1" low="1" first="1" last="1" negative="1" displayXAxis="0" displayHidden="0" minAxisType="group" maxAxisType="group" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
           <x14:colorSeries rgb="FF5F5F5F"/>
           <x14:colorNegative rgb="FFFFB620"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -3516,7 +3516,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" lineWeight="0.75" type="stacked" dateAxis="0" displayEmptyCellsAs="span" markers="0" high="1" low="1" first="1" last="1" negative="0" displayXAxis="0" displayHidden="0" minAxisType="individual" maxAxisType="individual" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
+        <x14:sparklineGroup lineWeight="0.75" type="stacked" dateAxis="0" displayEmptyCellsAs="span" markers="0" high="1" low="1" first="1" last="1" negative="0" displayXAxis="0" displayHidden="0" minAxisType="individual" maxAxisType="individual" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
           <x14:colorSeries rgb="FF5687C2"/>
           <x14:colorNegative rgb="FFFFB620"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -3540,7 +3540,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" manualMax="100" manualMin="-80" lineWeight="0.75" type="stacked" dateAxis="0" displayEmptyCellsAs="span" markers="1" high="0" low="0" first="0" last="0" negative="1" displayXAxis="0" displayHidden="0" minAxisType="custom" maxAxisType="custom" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
+        <x14:sparklineGroup manualMax="100" manualMin="-80" lineWeight="0.75" type="stacked" dateAxis="0" displayEmptyCellsAs="span" markers="1" high="0" low="0" first="0" last="0" negative="1" displayXAxis="0" displayHidden="0" minAxisType="custom" maxAxisType="custom" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
           <x14:colorSeries rgb="FFC6EFCE"/>
           <x14:colorNegative rgb="FFFFC7CE"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -3564,7 +3564,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" lineWeight="0.75" type="stacked" dateAxis="1" displayEmptyCellsAs="span" markers="0" high="0" low="0" first="0" last="0" negative="0" displayXAxis="0" displayHidden="0" minAxisType="individual" maxAxisType="individual" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
+        <x14:sparklineGroup lineWeight="0.75" type="stacked" dateAxis="1" displayEmptyCellsAs="span" markers="0" high="0" low="0" first="0" last="0" negative="0" displayXAxis="0" displayHidden="0" minAxisType="individual" maxAxisType="individual" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
           <x14:colorSeries rgb="FF5F5F5F"/>
           <x14:colorNegative rgb="FFFFB620"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -3589,7 +3589,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" lineWeight="2" type="stacked" dateAxis="0" displayEmptyCellsAs="span" markers="0" high="0" low="0" first="0" last="0" negative="0" displayXAxis="1" displayHidden="0" minAxisType="individual" maxAxisType="individual" rightToLeft="1" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
+        <x14:sparklineGroup lineWeight="2" type="stacked" dateAxis="0" displayEmptyCellsAs="span" markers="0" high="0" low="0" first="0" last="0" negative="0" displayXAxis="1" displayHidden="0" minAxisType="individual" maxAxisType="individual" rightToLeft="1" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
           <x14:colorSeries rgb="FF00B050"/>
           <x14:colorNegative rgb="FFFF0000"/>
           <x14:colorAxis rgb="FFFF0000"/>
@@ -3613,7 +3613,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" lineWeight="0.75" type="stacked" dateAxis="0" displayEmptyCellsAs="span" markers="0" high="0" low="0" first="1" last="1" negative="0" displayXAxis="0" displayHidden="0" minAxisType="individual" maxAxisType="individual" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
+        <x14:sparklineGroup lineWeight="0.75" type="stacked" dateAxis="0" displayEmptyCellsAs="span" markers="0" high="0" low="0" first="1" last="1" negative="0" displayXAxis="0" displayHidden="0" minAxisType="individual" maxAxisType="individual" rightToLeft="0" xr2:uid="{A98FF5F8-AE60-43B5-8001-AD89004F45D3}">
           <x14:colorSeries rgb="FFC6EFCE"/>
           <x14:colorNegative rgb="FFFFC7CE"/>
           <x14:colorAxis rgb="FF000000"/>

</xml_diff>